<commit_message>
updating to transition to home PC
</commit_message>
<xml_diff>
--- a/Project_Results_formatted.xlsx
+++ b/Project_Results_formatted.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mtmailmtsu-my.sharepoint.com/personal/mis2n_mtmail_mtsu_edu/Documents/NLP_ST/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mtmailmtsu-my.sharepoint.com/personal/mis2n_mtmail_mtsu_edu/Documents/Desktop/nlp_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71CEF095-6013-42DC-B39A-180BA2B7E02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{71CEF095-6013-42DC-B39A-180BA2B7E02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCB38EFE-B8CF-43BF-B14F-7519C611616F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12134,6 +12134,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E926"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A922" workbookViewId="0">
@@ -27888,5 +27891,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="52" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>